<commit_message>
Get parent info from the excel file
</commit_message>
<xml_diff>
--- a/course_notification.xlsx
+++ b/course_notification.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="student info" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="57">
   <si>
     <t xml:space="preserve">Student Name</t>
   </si>
@@ -31,7 +31,7 @@
     <t xml:space="preserve">Course</t>
   </si>
   <si>
-    <t xml:space="preserve">CLP Account Details</t>
+    <t xml:space="preserve">E-learning Account Details</t>
   </si>
   <si>
     <t xml:space="preserve">Google Meet Link</t>
@@ -114,6 +114,9 @@
     <t xml:space="preserve">Nguri Harrison</t>
   </si>
   <si>
+    <t xml:space="preserve">norulesanymore@gmail.com</t>
+  </si>
+  <si>
     <t xml:space="preserve">Rahima Nassir</t>
   </si>
   <si>
@@ -139,6 +142,9 @@
     <t xml:space="preserve">Nyamotai Nassir</t>
   </si>
   <si>
+    <t xml:space="preserve">bloodyrealme@gmail.com</t>
+  </si>
+  <si>
     <t xml:space="preserve">Annette Alen</t>
   </si>
   <si>
@@ -161,6 +167,9 @@
     <t xml:space="preserve">Alen Elema</t>
   </si>
   <si>
+    <t xml:space="preserve">harrison@tinkeredu.net</t>
+  </si>
+  <si>
     <t xml:space="preserve">Wilson Gitau</t>
   </si>
   <si>
@@ -183,6 +192,9 @@
     <t xml:space="preserve">Gitau Muchiri</t>
   </si>
   <si>
+    <t xml:space="preserve">harrisongitau3@gmail.com</t>
+  </si>
+  <si>
     <t xml:space="preserve">Natali Gichuru</t>
   </si>
   <si>
@@ -225,9 +237,6 @@
   </si>
   <si>
     <t xml:space="preserve">Lorrein Powell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wil</t>
   </si>
 </sst>
 </file>
@@ -313,7 +322,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -324,6 +333,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -343,10 +356,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+      <selection pane="topLeft" activeCell="K5" activeCellId="0" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -354,10 +367,12 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="32.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="48.9"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="6" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="27.09"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="1" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -411,146 +426,165 @@
       <c r="H2" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="I2" s="3" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H8" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" display="harry@somasoma.com"/>
     <hyperlink ref="E2" r:id="rId2" display="https://tel.meet/tfk-vqzw-kje?hs=5"/>
+    <hyperlink ref="I2" r:id="rId3" display="norulesanymore@gmail.com"/>
+    <hyperlink ref="I3" r:id="rId4" display="bloodyrealme@gmail.com"/>
+    <hyperlink ref="I4" r:id="rId5" display="harrison@tinkeredu.net"/>
+    <hyperlink ref="I5" r:id="rId6" display="harrisongitau3@gmail.com"/>
+    <hyperlink ref="I6" r:id="rId7" display="norulesanymore@gmail.com"/>
+    <hyperlink ref="I7" r:id="rId8" display="bloodyrealme@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>